<commit_message>
Destop - add more doc
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330371A5-A5D2-425A-A140-F550F08C3F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12375"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -434,14 +440,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,152 +449,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,7 +459,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.05"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,194 +469,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -823,251 +493,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1082,68 +510,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
@@ -1159,13 +543,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1201,13 +591,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:srcRect l="26410" t="20605" r="15897" b="21296"/>
         <a:stretch>
           <a:fillRect/>
@@ -1484,31 +880,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="32.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="14.7809523809524" customWidth="1"/>
-    <col min="5" max="5" width="17.6285714285714" customWidth="1"/>
-    <col min="6" max="6" width="21.1714285714286" customWidth="1"/>
-    <col min="7" max="7" width="10.552380952381" customWidth="1"/>
-    <col min="9" max="9" width="17.3904761904762" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1658,7 +1054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1681,7 +1077,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1704,7 +1100,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1727,7 +1123,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1747,7 +1143,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1770,7 +1166,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1781,7 +1177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -1805,7 +1201,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -1824,7 +1220,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
@@ -1849,7 +1245,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -2001,7 +1397,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2009,7 +1405,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2026,7 +1422,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -2043,7 +1439,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -2060,7 +1456,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -2078,25 +1474,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E44">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="E1:E44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2188,6 +1580,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Destop - add new Files
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330371A5-A5D2-425A-A140-F550F08C3F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB60F2B-9684-4856-B1F7-FA8054DD7711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="143">
   <si>
     <t>Arduino conentor</t>
   </si>
@@ -435,19 +435,50 @@
   </si>
   <si>
     <t>(Blanks)</t>
+  </si>
+  <si>
+    <t>4 Digital Output (PLC)</t>
+  </si>
+  <si>
+    <t>Voltage divider</t>
+  </si>
+  <si>
+    <t>Relay / Opto</t>
+  </si>
+  <si>
+    <t>PWM To Analog Converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0V-24V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0V-10V </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -499,7 +530,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -507,6 +538,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,8 +621,8 @@
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>359465</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -886,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -902,9 +939,12 @@
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -952,8 +992,17 @@
       <c r="K2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -978,8 +1027,14 @@
       <c r="K3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="M3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1004,8 +1059,14 @@
       <c r="K4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="M4" t="s">
+        <v>140</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1030,8 +1091,11 @@
       <c r="K5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="M5" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1054,7 +1118,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1100,7 +1164,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1123,7 +1187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1143,7 +1207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1166,7 +1230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1177,7 +1241,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -1201,7 +1265,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -1220,7 +1284,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
@@ -1245,7 +1309,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -1476,7 +1540,8 @@
   </sheetData>
   <autoFilter ref="E1:E44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1484,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Destop - test pwm to analog is done!!! Goodnight
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB60F2B-9684-4856-B1F7-FA8054DD7711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368DA4FF-0628-4856-AE9B-53452F41F401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="144">
   <si>
     <t>Arduino conentor</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t xml:space="preserve">0V-10V </t>
+  </si>
+  <si>
+    <t>1.37 Khz</t>
   </si>
 </sst>
 </file>
@@ -925,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1226,6 +1229,9 @@
       <c r="F11" t="s">
         <v>66</v>
       </c>
+      <c r="G11" t="s">
+        <v>143</v>
+      </c>
       <c r="H11" t="s">
         <v>67</v>
       </c>
@@ -1260,7 +1266,9 @@
       <c r="F13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>75</v>
       </c>
@@ -1549,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Destop - add more documents
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368DA4FF-0628-4856-AE9B-53452F41F401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF1B8EC-EFE2-47D3-8336-2C28337550DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,11 +480,25 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,8 +517,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -527,13 +552,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -543,15 +598,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -929,7 +995,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -971,25 +1037,26 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K2" t="s">
@@ -1006,25 +1073,26 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="K3" t="s">
@@ -1038,25 +1106,26 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="K4" t="s">
@@ -1070,25 +1139,26 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="K5" t="s">
@@ -1099,114 +1169,120 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a word file
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F7F5C2-2F53-4427-A8CF-8F2981DB296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A2C0A-C1A6-4E22-B534-5810EF3CD65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="Export List_STM32Peripheral" sheetId="3" r:id="rId2"/>
+    <sheet name="UML StateMachine" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pinout!$E$1:$E$44</definedName>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="167">
   <si>
     <t>STM32F469 Pinout</t>
   </si>
@@ -428,12 +428,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>(Blanks)</t>
-  </si>
-  <si>
     <t>4 Digital Output (PLC)</t>
   </si>
   <si>
@@ -468,31 +462,101 @@
   </si>
   <si>
     <t>Flow Sensor</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Screen::Menu</t>
+  </si>
+  <si>
+    <t>settingVarState</t>
+  </si>
+  <si>
+    <t>app::Main()</t>
+  </si>
+  <si>
+    <t>Screen::Setting</t>
+  </si>
+  <si>
+    <t>app::AdcStatup()</t>
+  </si>
+  <si>
+    <t>app::DigitalInStatup()</t>
+  </si>
+  <si>
+    <t>app::DigitalOutStatup()</t>
+  </si>
+  <si>
+    <t>app::PwmStatup()</t>
+  </si>
+  <si>
+    <t>app::AdcMain()</t>
+  </si>
+  <si>
+    <t>app::DigitalInMain()</t>
+  </si>
+  <si>
+    <t>app::DigitalOutMain()</t>
+  </si>
+  <si>
+    <t>app::PwmMain()</t>
+  </si>
+  <si>
+    <t>app::AdcExit()</t>
+  </si>
+  <si>
+    <t>app::DigitalInExit()</t>
+  </si>
+  <si>
+    <t>app::DigitalOutExit()</t>
+  </si>
+  <si>
+    <t>app::PwmExit()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -505,21 +569,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -527,7 +591,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -535,7 +599,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Bahnschrift SemiBold Condensed"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -640,20 +718,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
@@ -662,19 +740,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,16 +838,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>344805</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>162588</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>50358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>359465</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>63499</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>326335</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>121477</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -784,8 +871,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5921375" y="6850380"/>
-          <a:ext cx="10544175" cy="5976620"/>
+          <a:off x="10789175" y="6527358"/>
+          <a:ext cx="10566703" cy="5976619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1061,28 +1148,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
-    <col min="3" max="3" width="32.25" customWidth="1"/>
-    <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="10.625" customWidth="1"/>
-    <col min="9" max="9" width="17.375" customWidth="1"/>
-    <col min="11" max="11" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.25" customWidth="1"/>
-    <col min="13" max="13" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:15">
       <c r="A1" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1104,7 +1191,7 @@
       </c>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15">
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1131,16 +1218,16 @@
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15">
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1167,13 +1254,13 @@
         <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15">
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1200,10 +1287,10 @@
         <v>25</v>
       </c>
       <c r="M4" t="s">
+        <v>137</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1233,7 +1320,7 @@
         <v>31</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1374,7 +1461,7 @@
         <v>65</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>66</v>
@@ -1416,7 +1503,7 @@
         <v>65</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>74</v>
@@ -1719,7 +1806,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B27">
         <v>1501</v>
@@ -1732,17 +1819,17 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B33">
         <v>1502</v>
@@ -1757,104 +1844,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
+  <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
+    <row r="2" spans="2:5" ht="18.75">
+      <c r="B2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="D4" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="C8" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add function Suspend and Resume for apps
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F75DB4-A5DF-47B2-B548-41A59106CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49245F7C-5BB4-42A7-9DF5-4FEFF8E72CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="164">
   <si>
     <t>STM32F469 Pinout</t>
   </si>
@@ -488,56 +488,41 @@
     <t>app::Main()</t>
   </si>
   <si>
-    <t>Screen::Setting</t>
-  </si>
-  <si>
-    <t>app::AdcStatup()</t>
-  </si>
-  <si>
-    <t>app::DigitalInStatup()</t>
-  </si>
-  <si>
-    <t>app::DigitalOutStatup()</t>
-  </si>
-  <si>
-    <t>app::PwmStatup()</t>
-  </si>
-  <si>
-    <t>app::AdcMain()</t>
-  </si>
-  <si>
-    <t>app::DigitalInMain()</t>
-  </si>
-  <si>
-    <t>app::DigitalOutMain()</t>
-  </si>
-  <si>
-    <t>app::PwmMain()</t>
-  </si>
-  <si>
-    <t>app::AdcExit()</t>
-  </si>
-  <si>
-    <t>app::DigitalInExit()</t>
-  </si>
-  <si>
-    <t>app::DigitalOutExit()</t>
-  </si>
-  <si>
-    <t>app::PwmExit()</t>
-  </si>
-  <si>
     <t>PidGraph</t>
   </si>
   <si>
     <t>Screen::PidGraph</t>
+  </si>
+  <si>
+    <t>Function::settingVarState_entry()</t>
+  </si>
+  <si>
+    <t>Task::mainApp</t>
+  </si>
+  <si>
+    <t>Task::readAdc</t>
+  </si>
+  <si>
+    <t>Task::DdigitalIn</t>
+  </si>
+  <si>
+    <t>Task::DdigitalOut</t>
+  </si>
+  <si>
+    <t>Task::pwmUpdateCH0</t>
+  </si>
+  <si>
+    <t>Task::pwmUpdateCH1</t>
+  </si>
+  <si>
+    <t>Function::readAdcSuspend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +607,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -730,7 +721,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,6 +759,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1851,18 +1845,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75">
@@ -1896,68 +1890,57 @@
       <c r="B6" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" s="11"/>
+      <c r="D7" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="C8" s="11"/>
+      <c r="D8" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" s="11"/>
+      <c r="D10" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="D11" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="C7" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="C8" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="C9" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="C10" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all State machine is done
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2509635-68B7-44BF-AB31-D9EA1A6BA030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD55E379-2320-48E1-B4CA-5BF75918A54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="186">
   <si>
     <t>STM32F469 Pinout</t>
   </si>
@@ -626,6 +626,12 @@
       </rPr>
       <t>-&gt;notifyActualValueChanged()</t>
     </r>
+  </si>
+  <si>
+    <t>Function::PidComputingSuspend()</t>
+  </si>
+  <si>
+    <t>Function::PidComputingResume()</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2233,7 +2239,9 @@
     </row>
     <row r="21" spans="2:5" ht="18">
       <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="C21" s="19" t="s">
+        <v>184</v>
+      </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
     </row>
@@ -2281,9 +2289,13 @@
     </row>
     <row r="26" spans="2:5" ht="18">
       <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
+      <c r="C26" s="19" t="s">
+        <v>185</v>
+      </c>
       <c r="D26" s="25"/>
-      <c r="E26" s="21"/>
+      <c r="E26" s="21" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="27" spans="2:5" ht="18">
       <c r="B27" s="18" t="s">

</xml_diff>

<commit_message>
modify some wigget for more readability
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD55E379-2320-48E1-B4CA-5BF75918A54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5205719-73D7-4DA4-8574-DBA77A73AE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Fix bug, digital pin DO_2_PIN is wrong
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9B65AA-1770-4382-B792-A63EE38CD527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6611B0A-0B34-4299-8183-F1FF77CA4001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="205">
   <si>
     <t>STM32F469 Pinout</t>
   </si>
@@ -662,6 +662,33 @@
   </si>
   <si>
     <t>Hộp cảm biến V102</t>
+  </si>
+  <si>
+    <t>0V</t>
+  </si>
+  <si>
+    <t>đen</t>
+  </si>
+  <si>
+    <t>nâu</t>
+  </si>
+  <si>
+    <t>đỏ</t>
+  </si>
+  <si>
+    <t>lục</t>
+  </si>
+  <si>
+    <t>lam</t>
+  </si>
+  <si>
+    <t>tím</t>
+  </si>
+  <si>
+    <t>nâu trắng</t>
+  </si>
+  <si>
+    <t>đỏ trắng</t>
   </si>
 </sst>
 </file>
@@ -1376,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F10" activeCellId="1" sqref="B33 F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -2184,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
-  <dimension ref="B2:J48"/>
+  <dimension ref="B2:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -2197,15 +2224,13 @@
     <col min="3" max="3" width="51" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="10"/>
-    <col min="7" max="7" width="15.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="10"/>
+    <col min="6" max="6" width="2.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="3.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="2.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="20.25">
+    <row r="2" spans="2:19" ht="20.25">
       <c r="B2" s="14" t="s">
         <v>146</v>
       </c>
@@ -2218,32 +2243,109 @@
       <c r="E2" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="2:10" ht="18">
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>2</v>
+      </c>
+      <c r="I2" s="11">
+        <v>3</v>
+      </c>
+      <c r="J2" s="11">
+        <v>4</v>
+      </c>
+      <c r="K2" s="10">
+        <v>5</v>
+      </c>
+      <c r="L2" s="10">
+        <v>6</v>
+      </c>
+      <c r="M2" s="10">
+        <v>7</v>
+      </c>
+      <c r="O2" s="10">
+        <v>0</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1604</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="18">
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20"/>
       <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="2:10" ht="18">
+      <c r="G3" s="10">
+        <v>14</v>
+      </c>
+      <c r="H3" s="10">
+        <v>13</v>
+      </c>
+      <c r="I3" s="10">
+        <v>12</v>
+      </c>
+      <c r="J3" s="10">
+        <v>11</v>
+      </c>
+      <c r="K3" s="10">
+        <v>10</v>
+      </c>
+      <c r="L3" s="10">
+        <v>9</v>
+      </c>
+      <c r="M3" s="10">
+        <v>8</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1</v>
+      </c>
+      <c r="P3" s="10">
+        <v>1602</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="18">
       <c r="B4" s="22"/>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:10" ht="18">
+      <c r="O4" s="10">
+        <v>2</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>1601</v>
+      </c>
+      <c r="R4" s="10">
+        <v>1603</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="18">
       <c r="B5" s="22"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20"/>
       <c r="E5" s="21"/>
       <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:10" ht="18">
+      <c r="O5" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="18">
       <c r="B6" s="18" t="s">
         <v>151</v>
       </c>
@@ -2257,8 +2359,11 @@
         <v>159</v>
       </c>
       <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:10" ht="18">
+      <c r="O6" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="18">
       <c r="B7" s="22"/>
       <c r="C7" s="19" t="s">
         <v>166</v>
@@ -2270,8 +2375,23 @@
         <v>160</v>
       </c>
       <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:10" ht="18">
+      <c r="O7" s="10">
+        <v>5</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>1601</v>
+      </c>
+      <c r="R7" s="10">
+        <v>1603</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="18">
       <c r="B8" s="22"/>
       <c r="C8" s="19" t="s">
         <v>165</v>
@@ -2283,8 +2403,17 @@
         <v>161</v>
       </c>
       <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:10" ht="18">
+      <c r="O8" s="10">
+        <v>6</v>
+      </c>
+      <c r="P8" s="10">
+        <v>1505</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="18">
       <c r="B9" s="22"/>
       <c r="C9" s="19" t="s">
         <v>164</v>
@@ -2296,8 +2425,17 @@
         <v>163</v>
       </c>
       <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:10" ht="18">
+      <c r="O9" s="10">
+        <v>7</v>
+      </c>
+      <c r="P9" s="10">
+        <v>1501</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="18">
       <c r="B10" s="22"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
@@ -2305,8 +2443,17 @@
       </c>
       <c r="E10" s="21"/>
       <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:10" ht="18">
+      <c r="O10" s="10">
+        <v>8</v>
+      </c>
+      <c r="P10" s="10">
+        <v>1502</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="18">
       <c r="B11" s="22"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
@@ -2314,15 +2461,27 @@
       </c>
       <c r="E11" s="21"/>
       <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:10" ht="18">
+      <c r="O11" s="10">
+        <v>9</v>
+      </c>
+      <c r="P11" s="10">
+        <v>1506</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="18">
       <c r="B12" s="22"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
       <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:10" ht="18">
+      <c r="O12" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="18">
       <c r="B13" s="18" t="s">
         <v>168</v>
       </c>
@@ -2331,14 +2490,20 @@
         <v>169</v>
       </c>
       <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="2:10" ht="18">
+      <c r="O13" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" ht="18">
       <c r="B14" s="22"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="2:10" ht="18">
+      <c r="O14" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="18">
       <c r="B15" s="18" t="s">
         <v>150</v>
       </c>
@@ -2347,12 +2512,18 @@
         <v>153</v>
       </c>
       <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="2:10">
+      <c r="O15" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19">
       <c r="B16" s="24"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
+      <c r="O16" s="10">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="2:5" ht="18">
       <c r="B17" s="18" t="s">

</xml_diff>

<commit_message>
fixing too much, do not remember what i has done
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651073C7-3A9F-419F-948E-D6595C06CC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E2127A-391C-40F9-A7EB-55700E4629CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C33" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Bug send pid to backend
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E2127A-391C-40F9-A7EB-55700E4629CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837729FE-959E-43E9-8FA1-00AE16CD42BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="UML StateMachine" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="UML StateMachine" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pinout!$E$1:$E$44</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="215">
   <si>
     <t>STM32F469 Pinout</t>
   </si>
@@ -705,12 +706,27 @@
   <si>
     <t>LR.3.NO</t>
   </si>
+  <si>
+    <t>Pk</t>
+  </si>
+  <si>
+    <t>kI</t>
+  </si>
+  <si>
+    <t>kD</t>
+  </si>
+  <si>
+    <t>Kd = Kp * Td</t>
+  </si>
+  <si>
+    <t>Ki =Kp/Ti</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,6 +836,11 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="10">
@@ -952,7 +973,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1033,6 +1054,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1418,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C33" sqref="C32:C33"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -2245,6 +2269,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827E026E-B5C7-44A3-A29F-4B5D5F4ECE04}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="15" max="15" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="25.5">
+      <c r="O14" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="25.5">
+      <c r="O15" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3985EB97-567C-49AF-AA97-DA6EA7BC001D}">
   <dimension ref="B2:T48"/>
   <sheetViews>

</xml_diff>

<commit_message>
add zoom, forward, backward
</commit_message>
<xml_diff>
--- a/Doc/pinOut.xlsx
+++ b/Doc/pinOut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PCS_HMI\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCCD8D9-0981-4B1F-9690-E864B38AD55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1909FD2C-89DA-4E6C-ACC8-5CF5D4CC1FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -1470,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -2312,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827E026E-B5C7-44A3-A29F-4B5D5F4ECE04}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>